<commit_message>
Revision 2 - Final Turn in after udacity changes
</commit_message>
<xml_diff>
--- a/05 - Data Visualization/Visualization_Data_initial.xlsx
+++ b/05 - Data Visualization/Visualization_Data_initial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Code\School\WGU_DataAnalyst_NanoDegree\05 - Data Visualization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE534A8B-75A0-4B4B-B2E3-6319471FFA13}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F94BFD0-B3DC-4B04-975A-730F56FC8BE2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="675" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Orig_date</t>
+  </si>
+  <si>
+    <t>cluster_length</t>
   </si>
 </sst>
 </file>
@@ -511,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F83"/>
+  <dimension ref="A1:G83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,7 +527,7 @@
     <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -543,8 +546,11 @@
       <c r="F1" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>42397.829861111109</v>
       </c>
@@ -564,8 +570,12 @@
         <f>DATE(D2, MONTH(A2), DAY(A2))</f>
         <v>41667</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <f>COUNTIF(C:C, C2)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>42428.524305555547</v>
       </c>
@@ -585,8 +595,12 @@
         <f t="shared" ref="F3:F66" si="0">DATE(D3, MONTH(A3), DAY(A3))</f>
         <v>41698</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <f t="shared" ref="G3:G66" si="1">COUNTIF(C:C, C3)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>42430.856249999997</v>
       </c>
@@ -606,8 +620,12 @@
         <f t="shared" si="0"/>
         <v>41699</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>42442.259027777778</v>
       </c>
@@ -627,8 +645,12 @@
         <f t="shared" si="0"/>
         <v>41711</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>42447.763194444437</v>
       </c>
@@ -648,8 +670,12 @@
         <f t="shared" si="0"/>
         <v>41716</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>42465.012499999997</v>
       </c>
@@ -669,8 +695,12 @@
         <f t="shared" si="0"/>
         <v>41734</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>42486.459027777782</v>
       </c>
@@ -690,8 +720,12 @@
         <f t="shared" si="0"/>
         <v>41755</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>42517.717361111107</v>
       </c>
@@ -711,8 +745,12 @@
         <f t="shared" si="0"/>
         <v>41786</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>42526.347222222219</v>
       </c>
@@ -732,8 +770,12 @@
         <f t="shared" si="0"/>
         <v>41795</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>42542.879166666673</v>
       </c>
@@ -753,8 +795,12 @@
         <f t="shared" si="0"/>
         <v>41811</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>42544.821527777778</v>
       </c>
@@ -774,8 +820,12 @@
         <f t="shared" si="0"/>
         <v>41813</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>42577.154166666667</v>
       </c>
@@ -795,8 +845,12 @@
         <f t="shared" si="0"/>
         <v>41846</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>42582.286111111112</v>
       </c>
@@ -816,8 +870,12 @@
         <f t="shared" si="0"/>
         <v>41851</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>42590.415277777778</v>
       </c>
@@ -837,8 +895,12 @@
         <f t="shared" si="0"/>
         <v>41859</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>42707.085416666669</v>
       </c>
@@ -858,8 +920,12 @@
         <f t="shared" si="0"/>
         <v>41976</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>42722.479166666657</v>
       </c>
@@ -879,8 +945,12 @@
         <f t="shared" si="0"/>
         <v>41991</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>42406.798611111109</v>
       </c>
@@ -900,8 +970,12 @@
         <f t="shared" si="0"/>
         <v>42041</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>42421.886805555558</v>
       </c>
@@ -921,8 +995,12 @@
         <f t="shared" si="0"/>
         <v>42056</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>42486.304166666669</v>
       </c>
@@ -942,8 +1020,12 @@
         <f t="shared" si="0"/>
         <v>42120</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>42558.275694444441</v>
       </c>
@@ -963,8 +1045,12 @@
         <f t="shared" si="0"/>
         <v>42192</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>42565.905555555553</v>
       </c>
@@ -984,8 +1070,12 @@
         <f t="shared" si="0"/>
         <v>42199</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>42573.656944444447</v>
       </c>
@@ -1005,8 +1095,12 @@
         <f t="shared" si="0"/>
         <v>42207</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>42586.252083333333</v>
       </c>
@@ -1026,8 +1120,12 @@
         <f t="shared" si="0"/>
         <v>42220</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>42602.275694444441</v>
       </c>
@@ -1047,8 +1145,12 @@
         <f t="shared" si="0"/>
         <v>42236</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>42608.009722222218</v>
       </c>
@@ -1068,8 +1170,12 @@
         <f t="shared" si="0"/>
         <v>42242</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>42614.038194444453</v>
       </c>
@@ -1089,8 +1195,12 @@
         <f t="shared" si="0"/>
         <v>42248</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>42655.284722222219</v>
       </c>
@@ -1110,8 +1220,12 @@
         <f t="shared" si="0"/>
         <v>42289</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>42694.955555555563</v>
       </c>
@@ -1131,8 +1245,12 @@
         <f t="shared" si="0"/>
         <v>42328</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>42715.454861111109</v>
       </c>
@@ -1152,8 +1270,12 @@
         <f t="shared" si="0"/>
         <v>42349</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>42715.743055555547</v>
       </c>
@@ -1173,8 +1295,12 @@
         <f t="shared" si="0"/>
         <v>42349</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>42718.364583333343</v>
       </c>
@@ -1194,8 +1320,12 @@
         <f t="shared" si="0"/>
         <v>42352</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>42732.47152777778</v>
       </c>
@@ -1215,8 +1345,12 @@
         <f t="shared" si="0"/>
         <v>42366</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>42388.671527777777</v>
       </c>
@@ -1236,8 +1370,12 @@
         <f t="shared" si="0"/>
         <v>42388</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>42392.480555555558</v>
       </c>
@@ -1257,8 +1395,12 @@
         <f t="shared" si="0"/>
         <v>42392</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>42426.71875</v>
       </c>
@@ -1278,8 +1420,12 @@
         <f t="shared" si="0"/>
         <v>42426</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>42457.386111111111</v>
       </c>
@@ -1299,8 +1445,12 @@
         <f t="shared" si="0"/>
         <v>42457</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>42468.801388888889</v>
       </c>
@@ -1320,8 +1470,12 @@
         <f t="shared" si="0"/>
         <v>42468</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>42493.825694444437</v>
       </c>
@@ -1341,8 +1495,12 @@
         <f t="shared" si="0"/>
         <v>42493</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>42652.863888888889</v>
       </c>
@@ -1362,8 +1520,12 @@
         <f t="shared" si="0"/>
         <v>42652</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>42685.844444444447</v>
       </c>
@@ -1383,8 +1545,12 @@
         <f t="shared" si="0"/>
         <v>42685</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>42714.320833333331</v>
       </c>
@@ -1404,8 +1570,12 @@
         <f t="shared" si="0"/>
         <v>42714</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42720.479861111111</v>
       </c>
@@ -1425,8 +1595,12 @@
         <f t="shared" si="0"/>
         <v>42720</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>42371.775694444441</v>
       </c>
@@ -1446,8 +1620,12 @@
         <f t="shared" si="0"/>
         <v>42737</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>42387.276388888888</v>
       </c>
@@ -1467,8 +1645,12 @@
         <f t="shared" si="0"/>
         <v>42753</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>42455.905555555553</v>
       </c>
@@ -1488,8 +1670,12 @@
         <f t="shared" si="0"/>
         <v>42820</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>42457.397916666669</v>
       </c>
@@ -1509,8 +1695,12 @@
         <f t="shared" si="0"/>
         <v>42822</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G47">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>42493.842361111107</v>
       </c>
@@ -1530,8 +1720,12 @@
         <f t="shared" si="0"/>
         <v>42858</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>42501.915277777778</v>
       </c>
@@ -1551,8 +1745,12 @@
         <f t="shared" si="0"/>
         <v>42866</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>42518.547222222223</v>
       </c>
@@ -1572,8 +1770,12 @@
         <f t="shared" si="0"/>
         <v>42883</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G50">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>42519.842361111107</v>
       </c>
@@ -1593,8 +1795,12 @@
         <f t="shared" si="0"/>
         <v>42884</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G51">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>42537.9</v>
       </c>
@@ -1614,8 +1820,12 @@
         <f t="shared" si="0"/>
         <v>42902</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G52">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>42541.875694444447</v>
       </c>
@@ -1635,8 +1845,12 @@
         <f t="shared" si="0"/>
         <v>42906</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G53">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>42559.432638888888</v>
       </c>
@@ -1656,8 +1870,12 @@
         <f t="shared" si="0"/>
         <v>42924</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G54">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>42566.450694444437</v>
       </c>
@@ -1677,8 +1895,12 @@
         <f t="shared" si="0"/>
         <v>42931</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G55">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>42572.677083333343</v>
       </c>
@@ -1698,8 +1920,12 @@
         <f t="shared" si="0"/>
         <v>42937</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G56">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>42577.053472222222</v>
       </c>
@@ -1719,8 +1945,12 @@
         <f t="shared" si="0"/>
         <v>42942</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G57">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>42580.55</v>
       </c>
@@ -1740,8 +1970,12 @@
         <f t="shared" si="0"/>
         <v>42945</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G58">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>42584.353472222218</v>
       </c>
@@ -1761,8 +1995,12 @@
         <f t="shared" si="0"/>
         <v>42949</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G59">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>42635.05</v>
       </c>
@@ -1782,8 +2020,12 @@
         <f t="shared" si="0"/>
         <v>43000</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G60">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>42638.30972222222</v>
       </c>
@@ -1803,8 +2045,12 @@
         <f t="shared" si="0"/>
         <v>43003</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G61">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>42651.729861111111</v>
       </c>
@@ -1824,8 +2070,12 @@
         <f t="shared" si="0"/>
         <v>43016</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G62">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>42677.96875</v>
       </c>
@@ -1845,8 +2095,12 @@
         <f t="shared" si="0"/>
         <v>43042</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G63">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>42682.609722222223</v>
       </c>
@@ -1866,8 +2120,12 @@
         <f t="shared" si="0"/>
         <v>43047</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G64">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>42710.324305555558</v>
       </c>
@@ -1887,8 +2145,12 @@
         <f t="shared" si="0"/>
         <v>43075</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G65">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>42391.988888888889</v>
       </c>
@@ -1908,8 +2170,12 @@
         <f t="shared" si="0"/>
         <v>43122</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G66">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>42392.852083333331</v>
       </c>
@@ -1926,11 +2192,15 @@
         <v>17</v>
       </c>
       <c r="F67" s="3">
-        <f t="shared" ref="F67:F83" si="1">DATE(D67, MONTH(A67), DAY(A67))</f>
+        <f t="shared" ref="F67:F83" si="2">DATE(D67, MONTH(A67), DAY(A67))</f>
         <v>43123</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G67">
+        <f t="shared" ref="G67:G83" si="3">COUNTIF(C:C, C67)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>42403.468055555553</v>
       </c>
@@ -1947,11 +2217,15 @@
         <v>17</v>
       </c>
       <c r="F68" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43134</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G68">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>42455.373611111107</v>
       </c>
@@ -1968,11 +2242,15 @@
         <v>18</v>
       </c>
       <c r="F69" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43185</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G69">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>42463.072222222218</v>
       </c>
@@ -1989,11 +2267,15 @@
         <v>18</v>
       </c>
       <c r="F70" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43193</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G70">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>42499.804166666669</v>
       </c>
@@ -2010,11 +2292,15 @@
         <v>18</v>
       </c>
       <c r="F71" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43229</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G71">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>42526.897222222222</v>
       </c>
@@ -2031,11 +2317,15 @@
         <v>19</v>
       </c>
       <c r="F72" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43256</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G72">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>42532.059027777781</v>
       </c>
@@ -2052,11 +2342,15 @@
         <v>19</v>
       </c>
       <c r="F73" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43262</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G73">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>42546.9</v>
       </c>
@@ -2073,11 +2367,15 @@
         <v>19</v>
       </c>
       <c r="F74" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43276</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G74">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>42559.272222222222</v>
       </c>
@@ -2094,11 +2392,15 @@
         <v>19</v>
       </c>
       <c r="F75" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43289</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G75">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>42582.425000000003</v>
       </c>
@@ -2115,11 +2417,15 @@
         <v>19</v>
       </c>
       <c r="F76" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43312</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G76">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>42583.847916666673</v>
       </c>
@@ -2136,11 +2442,15 @@
         <v>19</v>
       </c>
       <c r="F77" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43313</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G77">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>42585.411805555559</v>
       </c>
@@ -2157,11 +2467,15 @@
         <v>19</v>
       </c>
       <c r="F78" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43315</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G78">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>42587.758333333331</v>
       </c>
@@ -2178,11 +2492,15 @@
         <v>19</v>
       </c>
       <c r="F79" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43317</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G79">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>42590.554166666669</v>
       </c>
@@ -2199,11 +2517,15 @@
         <v>19</v>
       </c>
       <c r="F80" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43320</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G80">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>42597.777083333327</v>
       </c>
@@ -2220,11 +2542,15 @@
         <v>19</v>
       </c>
       <c r="F81" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43327</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G81">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>42603.413194444453</v>
       </c>
@@ -2241,11 +2567,15 @@
         <v>19</v>
       </c>
       <c r="F82" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43333</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G82">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>42604.178472222222</v>
       </c>
@@ -2262,8 +2592,12 @@
         <v>19</v>
       </c>
       <c r="F83" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43334</v>
+      </c>
+      <c r="G83">
+        <f t="shared" si="3"/>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>